<commit_message>
eddy ni 1987-1988 (update 2)
</commit_message>
<xml_diff>
--- a/_data/ni/ni8788/individueel_eindstand_dworp_1234_8788.xlsx
+++ b/_data/ni/ni8788/individueel_eindstand_dworp_1234_8788.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="-15" windowWidth="14385" windowHeight="12870"/>
+    <workbookView xWindow="14340" yWindow="-15" windowWidth="14385" windowHeight="12870" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="272">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -253,12 +253,6 @@
     <t>De Smet Karl</t>
   </si>
   <si>
-    <t>Verlaenen R</t>
-  </si>
-  <si>
-    <t>Tournoy G</t>
-  </si>
-  <si>
     <t>Stiens Kris</t>
   </si>
   <si>
@@ -286,12 +280,6 @@
     <t>Flamee Dirk</t>
   </si>
   <si>
-    <t>Verzin</t>
-  </si>
-  <si>
-    <t>Werner G</t>
-  </si>
-  <si>
     <t>Roger Marc</t>
   </si>
   <si>
@@ -328,18 +316,6 @@
     <t>4E                 Westland werd uit competitie genomen, nul punten of algemeen forfait; niet 5,5 punten</t>
   </si>
   <si>
-    <t>Stuyts S</t>
-  </si>
-  <si>
-    <t>Noubaun</t>
-  </si>
-  <si>
-    <t>De Moerlooze</t>
-  </si>
-  <si>
-    <t>Meganck</t>
-  </si>
-  <si>
     <t>Furstenberg Tom</t>
   </si>
   <si>
@@ -388,9 +364,6 @@
     <t>216 Waterloo 1</t>
   </si>
   <si>
-    <t>402 JJ Gent 5</t>
-  </si>
-  <si>
     <t>245 Roque 5</t>
   </si>
   <si>
@@ -553,9 +526,6 @@
     <t>De Man Paul</t>
   </si>
   <si>
-    <t>De Weert Arnold</t>
-  </si>
-  <si>
     <t>Van Beurden Ben</t>
   </si>
   <si>
@@ -715,9 +685,6 @@
     <t>Roger Jean-Marie</t>
   </si>
   <si>
-    <t>Andrew, Ivan of Steve</t>
-  </si>
-  <si>
     <t>Delposen Alex</t>
   </si>
   <si>
@@ -787,12 +754,6 @@
     <t>Clayssens Jan</t>
   </si>
   <si>
-    <t>20338 Stuyts Simonne (kgsrl)</t>
-  </si>
-  <si>
-    <t>58700 Stuyts Jos (juiste niveau elo)</t>
-  </si>
-  <si>
     <t>De Merode Rodolphe</t>
   </si>
   <si>
@@ -808,12 +769,6 @@
     <t>Ruiz Berrocal Roberto</t>
   </si>
   <si>
-    <t>84166 Monbrun Thierry ?</t>
-  </si>
-  <si>
-    <t>82201 Demoerlooze Jaqueline (280) ?</t>
-  </si>
-  <si>
     <t>Van Roy Michel</t>
   </si>
   <si>
@@ -826,9 +781,6 @@
     <t>Lucke André</t>
   </si>
   <si>
-    <t>84158 Makanga Charles ???</t>
-  </si>
-  <si>
     <t>14;8</t>
   </si>
   <si>
@@ -839,6 +791,57 @@
   </si>
   <si>
     <t>22,5;13</t>
+  </si>
+  <si>
+    <t>Werner Guy</t>
+  </si>
+  <si>
+    <t>De Weerdt Arnold</t>
+  </si>
+  <si>
+    <t>Waroquier in nota's van Eddy</t>
+  </si>
+  <si>
+    <t>Ivan (1568 elo sept '87) of Steve (1446 elo sept '87)</t>
+  </si>
+  <si>
+    <t>Stuyts Jos</t>
+  </si>
+  <si>
+    <t>In Eddy zijn notities staat "Stuyts S"</t>
+  </si>
+  <si>
+    <t>58700 Stuyts Jos (1894 elo sept '87)</t>
+  </si>
+  <si>
+    <t>20338 Stuyts Simonne (1576 elo in sept '87))</t>
+  </si>
+  <si>
+    <t>402 Jean Jaurès Gent 5</t>
+  </si>
+  <si>
+    <t>Monbrun Thierry</t>
+  </si>
+  <si>
+    <t>De Moerlooze Jacqueline</t>
+  </si>
+  <si>
+    <t>82201 Demoerlooze Jaqueline (club 501 in '87, club 280 in '89) ?</t>
+  </si>
+  <si>
+    <t>Meganck Marc</t>
+  </si>
+  <si>
+    <t>Monbrun ipv. "Noubaun" ? Dat zijn 3 letters verschil, maar wel letters die geschreven op elkaar kunnen lijken: N -&gt; M, u -&gt; n, a -&gt; r.  Noubaun is nergens terug te vinden.</t>
+  </si>
+  <si>
+    <t>In het eloklassement van sept '87 (de basis van de spelerslijsten) staat De Moerlooze Jacqueline elo 1146 kring 501 Charleroi. Het feit dat ze won tegen De Wilde sterkt mij in de overtuiging dat zij voor Pantin speelde. Met 1146 elo moest ze op het eerste bord spelen; als enige uitzondering zou de regel kunnen bestaan dat het een voorlopige quotering was (= tussen 10 en 20 partijen verwerkt).</t>
+  </si>
+  <si>
+    <t>In het eloklassement van sept '87 (de basis van de spelerslijsten) staat Meganck Marc elo 0 kring 274 Westland Chess Club (bron: CEFB mars 1987) stamnummer 88706.</t>
+  </si>
+  <si>
+    <t>vanaf januari '90 staat Marc Meganck op de elolijst van Pantin</t>
   </si>
 </sst>
 </file>
@@ -1506,7 +1509,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1774,6 +1777,7 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2077,7 +2081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2095,7 +2099,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1">
       <c r="A2" s="68" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2125,7 +2129,7 @@
         <v>1988</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
@@ -2147,7 +2151,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
@@ -2175,7 +2179,7 @@
         <v>59</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -2188,11 +2192,11 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1">
       <c r="A9" s="76" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B9" s="77"/>
       <c r="D9" s="61" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -2205,7 +2209,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="78" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B10" s="79">
         <v>0</v>
@@ -2213,7 +2217,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="78" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B11" s="80">
         <v>1</v>
@@ -2221,13 +2225,13 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1">
       <c r="A12" s="78" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B12" s="81">
         <v>0</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E12" s="65"/>
       <c r="F12" s="65"/>
@@ -2238,7 +2242,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="D13" s="65" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E13" s="65"/>
       <c r="F13" s="65"/>
@@ -2249,7 +2253,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="D15" s="64" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="64"/>
@@ -2311,7 +2315,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2321,7 +2325,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -2377,7 +2381,7 @@
         <v>8877</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -2403,7 +2407,7 @@
         <v>28398</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -2429,7 +2433,7 @@
         <v>71005</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -2455,7 +2459,7 @@
         <v>2526</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -2481,7 +2485,7 @@
         <v>27928</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -2507,7 +2511,7 @@
         <v>42200</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -2542,7 +2546,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2552,7 +2556,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -2608,7 +2612,7 @@
         <v>18988</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -2634,7 +2638,7 @@
         <v>17523</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -2660,7 +2664,7 @@
         <v>83585</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -2686,7 +2690,7 @@
         <v>85201</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -2721,7 +2725,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2731,7 +2735,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="93" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -2771,7 +2775,7 @@
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="10"/>
@@ -2783,7 +2787,7 @@
         <v>9270</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J23" s="18">
         <v>1772</v>
@@ -2795,7 +2799,7 @@
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="10"/>
@@ -2807,7 +2811,7 @@
         <v>64327</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J24" s="18">
         <v>1616</v>
@@ -2819,7 +2823,7 @@
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="10"/>
@@ -2843,7 +2847,7 @@
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="12"/>
@@ -2892,7 +2896,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -2902,7 +2906,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="93" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -2942,7 +2946,7 @@
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="10"/>
@@ -2966,7 +2970,7 @@
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="10"/>
@@ -2990,7 +2994,7 @@
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="10"/>
@@ -3014,7 +3018,7 @@
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="12"/>
@@ -4282,7 +4286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD280"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4311,13 +4315,13 @@
         <v>14</v>
       </c>
       <c r="S2" s="82" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="AF2" s="83" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="AS2" s="82" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:56" s="43" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
@@ -4402,7 +4406,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>37</v>
@@ -4596,7 +4600,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C5" s="34">
         <v>4</v>
@@ -4790,7 +4794,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C6" s="34">
         <v>2</v>
@@ -4984,7 +4988,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C7" s="34">
         <v>1.5</v>
@@ -5178,7 +5182,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C8" s="34">
         <v>1</v>
@@ -5372,7 +5376,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C9" s="34">
         <v>2</v>
@@ -5566,7 +5570,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C10" s="34">
         <v>2.5</v>
@@ -5760,7 +5764,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C11" s="34">
         <v>1.5</v>
@@ -5954,7 +5958,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C12" s="34">
         <v>1.5</v>
@@ -6148,7 +6152,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C13" s="34">
         <v>2</v>
@@ -6784,7 +6788,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>37</v>
@@ -6978,7 +6982,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C19" s="34">
         <v>1.5</v>
@@ -7172,7 +7176,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>120</v>
+        <v>263</v>
       </c>
       <c r="C20" s="34">
         <v>1.5</v>
@@ -7366,7 +7370,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C21" s="34">
         <v>2.5</v>
@@ -7560,7 +7564,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C22" s="34">
         <v>2</v>
@@ -7754,7 +7758,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C23" s="34">
         <v>0.5</v>
@@ -7948,7 +7952,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C24" s="34">
         <v>2</v>
@@ -8142,7 +8146,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C25" s="34">
         <v>1</v>
@@ -8336,7 +8340,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C26" s="34">
         <v>1.5</v>
@@ -8530,7 +8534,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C27" s="102">
         <v>0.5</v>
@@ -9165,7 +9169,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C32" s="33" t="s">
         <v>37</v>
@@ -9208,7 +9212,7 @@
         <v>7</v>
       </c>
       <c r="R32" s="100" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="S32" s="46" t="s">
         <v>37</v>
@@ -9357,7 +9361,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C33" s="98">
         <v>2</v>
@@ -9400,7 +9404,7 @@
         <v>7</v>
       </c>
       <c r="R33" s="100" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="S33" s="47">
         <f>IF(C33="","",IF(C33&gt;D32,1,IF(C33=D32,0.5,0)))</f>
@@ -9549,7 +9553,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C34" s="66">
         <v>1</v>
@@ -9739,7 +9743,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C35" s="98">
         <v>1</v>
@@ -9929,7 +9933,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C36" s="98">
         <v>0</v>
@@ -10119,7 +10123,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C37" s="98">
         <v>0.5</v>
@@ -10162,7 +10166,7 @@
         <v>7</v>
       </c>
       <c r="R37" s="100" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="S37" s="47">
         <f>IF(C37="","",IF(C37&gt;$H32,1,IF(C37=$H32,0.5,0)))</f>
@@ -10311,7 +10315,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C38" s="96">
         <v>0</v>
@@ -10354,7 +10358,7 @@
         <v>7</v>
       </c>
       <c r="R38" s="100" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="S38" s="47">
         <f>IF(C38="","",IF(C38&gt;$I32,1,IF(C38=$I32,0.5,0)))</f>
@@ -10503,7 +10507,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C39" s="66">
         <v>0</v>
@@ -11483,7 +11487,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>37</v>
@@ -11673,7 +11677,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C47" s="34">
         <v>1.5</v>
@@ -11863,7 +11867,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C48" s="34">
         <v>0</v>
@@ -12053,7 +12057,7 @@
         <v>4</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C49" s="34">
         <v>0</v>
@@ -12243,7 +12247,7 @@
         <v>5</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C50" s="34">
         <v>0</v>
@@ -12433,7 +12437,7 @@
         <v>6</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C51" s="34">
         <v>1</v>
@@ -12623,7 +12627,7 @@
         <v>7</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C52" s="34">
         <v>0.5</v>
@@ -12813,7 +12817,7 @@
         <v>8</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C53" s="34">
         <v>0</v>
@@ -16826,7 +16830,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16866,7 +16870,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -16876,7 +16880,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -16918,7 +16922,7 @@
         <v>63011</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -16948,7 +16952,7 @@
         <v>58432</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -16978,7 +16982,7 @@
         <v>24872</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -17000,7 +17004,7 @@
         <v>2021</v>
       </c>
       <c r="L7" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -17011,7 +17015,7 @@
         <v>60038</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -17041,7 +17045,7 @@
         <v>28207</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -17071,7 +17075,7 @@
         <v>9130</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -17128,7 +17132,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -17138,7 +17142,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -17240,7 +17244,7 @@
         <v>73067</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -17270,7 +17274,7 @@
         <v>69540</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -17327,7 +17331,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -17337,7 +17341,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="93" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -17379,7 +17383,7 @@
         <v>83089</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="10">
@@ -17409,7 +17413,7 @@
         <v>72761</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="10">
@@ -17439,7 +17443,7 @@
         <v>90417</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="10">
@@ -17469,7 +17473,7 @@
         <v>53813</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="12">
@@ -17526,7 +17530,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -17536,7 +17540,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="93" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -17578,7 +17582,7 @@
         <v>38245</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="10">
@@ -17608,7 +17612,7 @@
         <v>94439</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>175</v>
+        <v>256</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="10">
@@ -17638,7 +17642,7 @@
         <v>48461</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="10">
@@ -17668,7 +17672,7 @@
         <v>23426</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="12">
@@ -17690,7 +17694,7 @@
         <v>73</v>
       </c>
       <c r="L34" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -17768,7 +17772,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -17778,7 +17782,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -17840,7 +17844,7 @@
         <v>77038</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -17930,7 +17934,7 @@
         <v>35386</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -17960,7 +17964,7 @@
         <v>75418</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -17990,7 +17994,7 @@
         <v>67814</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -18029,7 +18033,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -18039,7 +18043,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -18099,7 +18103,7 @@
         <v>55611</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -18129,7 +18133,7 @@
         <v>55603</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -18159,7 +18163,7 @@
         <v>77259</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -18189,11 +18193,11 @@
         <v>72371</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="J18" s="18"/>
       <c r="L18" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -18231,7 +18235,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="93" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -18241,7 +18245,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -18391,7 +18395,7 @@
         <v>9989</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="J26" s="18"/>
     </row>
@@ -18430,7 +18434,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="93" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -18440,7 +18444,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -18500,7 +18504,7 @@
         <v>90051</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="J31" s="18"/>
     </row>
@@ -18560,7 +18564,7 @@
         <v>16721</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="J33" s="18"/>
     </row>
@@ -18590,7 +18594,7 @@
         <v>22951</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="J34" s="18"/>
     </row>
@@ -18669,7 +18673,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -18679,7 +18683,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -18721,7 +18725,7 @@
         <v>1473</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -18751,7 +18755,7 @@
         <v>92894</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -18781,7 +18785,7 @@
         <v>591</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -18811,7 +18815,7 @@
         <v>1287</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -18841,7 +18845,7 @@
         <v>1465</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -18871,7 +18875,7 @@
         <v>84310</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -18928,7 +18932,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -18938,7 +18942,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -18980,7 +18984,7 @@
         <v>50377</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -19010,7 +19014,7 @@
         <v>61158</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -19070,7 +19074,7 @@
         <v>87823</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -19127,7 +19131,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -19137,7 +19141,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="93" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -19179,7 +19183,7 @@
         <v>31241</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="10">
@@ -19209,7 +19213,7 @@
         <v>33430</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="10">
@@ -19239,7 +19243,7 @@
         <v>41769</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="10">
@@ -19269,7 +19273,7 @@
         <v>41785</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="12">
@@ -19285,7 +19289,7 @@
         <v>95707</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J26" s="18">
         <v>1565</v>
@@ -19326,7 +19330,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -19336,7 +19340,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="93" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -19378,7 +19382,7 @@
         <v>38857</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="10">
@@ -19408,7 +19412,7 @@
         <v>95486</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="10">
@@ -19438,7 +19442,7 @@
         <v>40703</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="10">
@@ -19468,7 +19472,7 @@
         <v>25992</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="12">
@@ -19565,7 +19569,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -19575,7 +19579,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -19635,7 +19639,7 @@
         <v>17647</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -19665,7 +19669,7 @@
         <v>43702</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -19695,7 +19699,7 @@
         <v>31259</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -19725,7 +19729,7 @@
         <v>62286</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -19755,7 +19759,7 @@
         <v>9563</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -19785,7 +19789,7 @@
         <v>52850</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -19824,7 +19828,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -19834,7 +19838,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -19894,7 +19898,7 @@
         <v>604</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -19924,7 +19928,7 @@
         <v>27987</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -19954,7 +19958,7 @@
         <v>96506</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -19984,7 +19988,7 @@
         <v>41688</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -20023,7 +20027,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -20033,7 +20037,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="93" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -20075,7 +20079,7 @@
         <v>17663</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="10">
@@ -20105,7 +20109,7 @@
         <v>80179</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="10">
@@ -20121,7 +20125,7 @@
         <v>64327</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J24" s="18">
         <v>1616</v>
@@ -20135,7 +20139,7 @@
         <v>64408</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="10">
@@ -20151,7 +20155,7 @@
         <v>95707</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J25" s="18">
         <v>1565</v>
@@ -20165,7 +20169,7 @@
         <v>59668</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="12">
@@ -20222,7 +20226,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -20232,7 +20236,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="93" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -20274,7 +20278,7 @@
         <v>87904</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="10">
@@ -20304,7 +20308,7 @@
         <v>9873</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="10">
@@ -20326,7 +20330,7 @@
         <v>1848</v>
       </c>
       <c r="L32" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -20337,7 +20341,7 @@
         <v>20362</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="10">
@@ -20367,7 +20371,7 @@
         <v>4502</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="12">
@@ -20424,7 +20428,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20464,7 +20468,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -20474,7 +20478,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -20516,7 +20520,7 @@
         <v>42161</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -20546,7 +20550,7 @@
         <v>19267</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -20576,7 +20580,7 @@
         <v>19208</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -20606,7 +20610,7 @@
         <v>49956</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -20636,7 +20640,7 @@
         <v>19135</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -20666,7 +20670,7 @@
         <v>76244</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -20723,7 +20727,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -20733,7 +20737,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -20771,9 +20775,11 @@
       <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="19">
+        <v>17663</v>
+      </c>
       <c r="C15" s="14" t="s">
-        <v>86</v>
+        <v>212</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -20799,9 +20805,11 @@
       <c r="A16" s="5">
         <v>2</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="19">
+        <v>80179</v>
+      </c>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>213</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -20827,9 +20835,11 @@
       <c r="A17" s="5">
         <v>3</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="19">
+        <v>64408</v>
+      </c>
       <c r="C17" s="14" t="s">
-        <v>76</v>
+        <v>214</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -20855,9 +20865,11 @@
       <c r="A18" s="5">
         <v>4</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="19">
+        <v>45365</v>
+      </c>
       <c r="C18" s="14" t="s">
-        <v>87</v>
+        <v>255</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -21183,8 +21195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21224,7 +21236,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -21234,7 +21246,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -21294,7 +21306,7 @@
         <v>39471</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -21324,7 +21336,7 @@
         <v>72397</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -21354,7 +21366,7 @@
         <v>75990</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -21384,7 +21396,7 @@
         <v>78123</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -21414,9 +21426,11 @@
         <v>72389</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="J9" s="18"/>
+        <v>218</v>
+      </c>
+      <c r="J9" s="18">
+        <v>1667</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1">
       <c r="A10" s="5">
@@ -21442,11 +21456,11 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J10" s="18"/>
       <c r="L10" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -21467,9 +21481,9 @@
         <v>2.5</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="16" t="str">
+      <c r="I11" s="16">
         <f>IFERROR(AVERAGE(J5:J10),"")</f>
-        <v/>
+        <v>1667</v>
       </c>
       <c r="J11" s="3"/>
     </row>
@@ -21484,7 +21498,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -21494,7 +21508,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -21542,7 +21556,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -21560,7 +21574,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -21578,7 +21592,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -21596,7 +21610,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -21943,7 +21957,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -21953,7 +21967,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -21995,7 +22009,7 @@
         <v>5606</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -22017,7 +22031,7 @@
         <v>2121</v>
       </c>
       <c r="L5" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -22028,7 +22042,7 @@
         <v>80489</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -22058,7 +22072,7 @@
         <v>92002</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -22088,7 +22102,7 @@
         <v>67440</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -22118,7 +22132,7 @@
         <v>69311</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -22148,7 +22162,7 @@
         <v>12122</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -22205,7 +22219,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -22215,7 +22229,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -22257,7 +22271,7 @@
         <v>30881</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -22287,7 +22301,7 @@
         <v>45292</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -22317,7 +22331,7 @@
         <v>30856</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -22347,7 +22361,7 @@
         <v>25453</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -22404,7 +22418,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="93" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -22414,7 +22428,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -22474,7 +22488,7 @@
         <v>75141</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="J23" s="18"/>
     </row>
@@ -22504,7 +22518,7 @@
         <v>29289</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="J24" s="18"/>
     </row>
@@ -22534,7 +22548,7 @@
         <v>84565</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="J25" s="18"/>
     </row>
@@ -22546,7 +22560,7 @@
         <v>95707</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26" s="18">
         <v>1565</v>
@@ -22564,7 +22578,7 @@
         <v>75175</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="J26" s="18"/>
     </row>
@@ -22603,7 +22617,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="93" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -22613,7 +22627,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -22673,7 +22687,7 @@
         <v>74233</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="J31" s="18"/>
     </row>
@@ -22703,7 +22717,7 @@
         <v>19321</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="J32" s="18"/>
     </row>
@@ -22733,7 +22747,7 @@
         <v>19615</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J33" s="18"/>
     </row>
@@ -22763,7 +22777,7 @@
         <v>36447</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J34" s="18"/>
     </row>
@@ -22801,8 +22815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22820,7 +22834,7 @@
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21">
+    <row r="1" spans="1:12" ht="21">
       <c r="A1" s="23" t="s">
         <v>27</v>
       </c>
@@ -22831,18 +22845,18 @@
         <v>32208</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19.5" thickBot="1">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -22852,11 +22866,11 @@
         <v>12</v>
       </c>
       <c r="I3" s="93" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -22886,7 +22900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -22894,7 +22908,7 @@
         <v>54810</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -22916,7 +22930,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -22924,7 +22938,7 @@
         <v>19933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -22946,7 +22960,7 @@
         <v>2101</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -22954,7 +22968,7 @@
         <v>5720</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -22976,7 +22990,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -22984,7 +22998,7 @@
         <v>12157</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -23006,7 +23020,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:12">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -23014,7 +23028,7 @@
         <v>68721</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -23036,7 +23050,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -23044,7 +23058,7 @@
         <v>65765</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -23065,8 +23079,11 @@
       <c r="J10" s="18">
         <v>1686</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="16" t="str">
@@ -23090,18 +23107,18 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="19.5" thickBot="1">
+    <row r="12" spans="1:12" ht="19.5" thickBot="1">
       <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:12">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>120</v>
+        <v>263</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -23111,11 +23128,11 @@
         <v>12</v>
       </c>
       <c r="I13" s="93" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:12">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -23145,7 +23162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:12">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -23153,7 +23170,7 @@
         <v>3701</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -23175,7 +23192,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:12">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -23183,9 +23200,11 @@
         <v>16748</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="D16" s="18"/>
+        <v>239</v>
+      </c>
+      <c r="D16" s="18">
+        <v>1896</v>
+      </c>
       <c r="E16" s="10">
         <v>1</v>
       </c>
@@ -23203,17 +23222,24 @@
       </c>
       <c r="J16" s="18">
         <v>1920</v>
+      </c>
+      <c r="L16" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="5">
         <v>3</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="19">
+        <v>58700</v>
+      </c>
       <c r="C17" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="18"/>
+        <v>259</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1894</v>
+      </c>
       <c r="E17" s="10">
         <v>0.5</v>
       </c>
@@ -23233,7 +23259,7 @@
         <v>1892</v>
       </c>
       <c r="L17" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1">
@@ -23244,9 +23270,11 @@
         <v>16675</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D18" s="18"/>
+        <v>240</v>
+      </c>
+      <c r="D18" s="18">
+        <v>1881</v>
+      </c>
       <c r="E18" s="12">
         <v>0.5</v>
       </c>
@@ -23266,15 +23294,15 @@
         <v>1874</v>
       </c>
       <c r="L18" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A19" s="6"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="16" t="str">
+      <c r="C19" s="16">
         <f>IFERROR(AVERAGE(D15:D18),"")</f>
-        <v/>
+        <v>1890.3333333333333</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="13">
@@ -23304,7 +23332,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="93" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -23314,7 +23342,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -23370,13 +23398,17 @@
       <c r="G23" s="10">
         <v>1</v>
       </c>
-      <c r="H23" s="19"/>
+      <c r="H23" s="19">
+        <v>84166</v>
+      </c>
       <c r="I23" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="J23" s="18"/>
+        <v>264</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="L23" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -23387,7 +23419,7 @@
         <v>64327</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D24" s="18">
         <v>1616</v>
@@ -23405,9 +23437,14 @@
         <v>89460</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="J24" s="18"/>
+        <v>242</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="5">
@@ -23431,13 +23468,17 @@
       <c r="G25" s="10">
         <v>1</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="19">
+        <v>82201</v>
+      </c>
       <c r="I25" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="18"/>
-      <c r="L25" t="s">
-        <v>261</v>
+        <v>265</v>
+      </c>
+      <c r="J25" s="18">
+        <v>1146</v>
+      </c>
+      <c r="L25" s="103" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
@@ -23462,13 +23503,17 @@
       <c r="G26" s="12">
         <v>1</v>
       </c>
-      <c r="H26" s="19"/>
+      <c r="H26" s="19">
+        <v>88706</v>
+      </c>
       <c r="I26" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" s="18"/>
+        <v>267</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="L26" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -23489,11 +23534,14 @@
         <v>4</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="16" t="str">
+      <c r="I27" s="16">
         <f>IFERROR(AVERAGE(J23:J26),"")</f>
-        <v/>
+        <v>1146</v>
       </c>
       <c r="J27" s="3"/>
+      <c r="L27" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">
       <c r="A28" s="17" t="s">
@@ -23506,7 +23554,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="93" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -23516,7 +23564,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -23576,7 +23624,7 @@
         <v>90293</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="J31" s="18"/>
     </row>
@@ -23606,7 +23654,7 @@
         <v>90247</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="J32" s="18"/>
     </row>
@@ -23636,7 +23684,7 @@
         <v>90221</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="J33" s="18"/>
     </row>
@@ -23666,7 +23714,7 @@
         <v>90255</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="J34" s="18"/>
     </row>

</xml_diff>

<commit_message>
eddy ni 1987-1988 (update 3)
</commit_message>
<xml_diff>
--- a/_data/ni/ni8788/individueel_eindstand_dworp_1234_8788.xlsx
+++ b/_data/ni/ni8788/individueel_eindstand_dworp_1234_8788.xlsx
@@ -790,9 +790,6 @@
     <t>11,5;6</t>
   </si>
   <si>
-    <t>22,5;13</t>
-  </si>
-  <si>
     <t>Werner Guy</t>
   </si>
   <si>
@@ -842,6 +839,9 @@
   </si>
   <si>
     <t>vanaf januari '90 staat Marc Meganck op de elolijst van Pantin</t>
+  </si>
+  <si>
+    <t>8?</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1509,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1778,6 +1778,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="11" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4286,7 +4292,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD280"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7176,7 +7184,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C20" s="34">
         <v>1.5</v>
@@ -7796,7 +7804,7 @@
         <f t="shared" si="6"/>
         <v>19.5</v>
       </c>
-      <c r="P23" s="36">
+      <c r="P23" s="97">
         <f>IF(Info!B$10=0,0,SUM(S23:AD23))+IF(Info!B$11=0,0,2*SUM(S23:AD23))+IF(Info!B$12=0,0,SUM(AS23:BD23))</f>
         <v>9</v>
       </c>
@@ -7804,7 +7812,9 @@
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="R23" s="45"/>
+      <c r="R23" s="100" t="s">
+        <v>271</v>
+      </c>
       <c r="S23" s="47">
         <f>IF(C23="","",IF(C23&gt;$H18,1,IF(C23=$H18,0.5,0)))</f>
         <v>0</v>
@@ -9177,7 +9187,7 @@
       <c r="D32" s="98">
         <v>2</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="34">
         <v>3</v>
       </c>
       <c r="F32" s="98">
@@ -9192,7 +9202,7 @@
       <c r="I32" s="34">
         <v>4</v>
       </c>
-      <c r="J32" s="66">
+      <c r="J32" s="34">
         <v>4</v>
       </c>
       <c r="K32" s="34"/>
@@ -9203,7 +9213,7 @@
         <f t="shared" ref="O32:O43" si="11">SUM(C32:N32)</f>
         <v>23.5</v>
       </c>
-      <c r="P32" s="36">
+      <c r="P32" s="104">
         <f>IF(Info!B$10=0,0,SUM(S32:AD32))+IF(Info!B$11=0,0,2*SUM(S32:AD32))+IF(Info!B$12=0,0,SUM(AS32:BD32))</f>
         <v>13</v>
       </c>
@@ -9211,8 +9221,8 @@
         <f t="shared" ref="Q32:Q43" si="12">COUNT(C32:N32)</f>
         <v>7</v>
       </c>
-      <c r="R32" s="100" t="s">
-        <v>254</v>
+      <c r="R32" s="100">
+        <v>22.5</v>
       </c>
       <c r="S32" s="46" t="s">
         <v>37</v>
@@ -9372,7 +9382,7 @@
       <c r="E33" s="98">
         <v>1.5</v>
       </c>
-      <c r="F33" s="66">
+      <c r="F33" s="34">
         <v>2.5</v>
       </c>
       <c r="G33" s="98">
@@ -9384,7 +9394,7 @@
       <c r="I33" s="67">
         <v>3.5</v>
       </c>
-      <c r="J33" s="66">
+      <c r="J33" s="34">
         <v>4</v>
       </c>
       <c r="K33" s="34"/>
@@ -9583,11 +9593,11 @@
       <c r="L34" s="34"/>
       <c r="M34" s="34"/>
       <c r="N34" s="34"/>
-      <c r="O34" s="35">
+      <c r="O34" s="105">
         <f t="shared" si="11"/>
         <v>17.5</v>
       </c>
-      <c r="P34" s="36">
+      <c r="P34" s="104">
         <f>IF(Info!B$10=0,0,SUM(S34:AD34))+IF(Info!B$11=0,0,2*SUM(S34:AD34))+IF(Info!B$12=0,0,SUM(AS34:BD34))</f>
         <v>10</v>
       </c>
@@ -9773,11 +9783,11 @@
       <c r="L35" s="34"/>
       <c r="M35" s="34"/>
       <c r="N35" s="34"/>
-      <c r="O35" s="35">
+      <c r="O35" s="105">
         <f t="shared" si="11"/>
         <v>16.5</v>
       </c>
-      <c r="P35" s="36">
+      <c r="P35" s="104">
         <f>IF(Info!B$10=0,0,SUM(S35:AD35))+IF(Info!B$11=0,0,2*SUM(S35:AD35))+IF(Info!B$12=0,0,SUM(AS35:BD35))</f>
         <v>9</v>
       </c>
@@ -9963,11 +9973,11 @@
       <c r="L36" s="34"/>
       <c r="M36" s="34"/>
       <c r="N36" s="34"/>
-      <c r="O36" s="35">
+      <c r="O36" s="105">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="P36" s="36">
+      <c r="P36" s="104">
         <f>IF(Info!B$10=0,0,SUM(S36:AD36))+IF(Info!B$11=0,0,2*SUM(S36:AD36))+IF(Info!B$12=0,0,SUM(AS36:BD36))</f>
         <v>6</v>
       </c>
@@ -10137,7 +10147,7 @@
       <c r="F37" s="98">
         <v>1.5</v>
       </c>
-      <c r="G37" s="66">
+      <c r="G37" s="34">
         <v>1</v>
       </c>
       <c r="H37" s="33" t="s">
@@ -10329,7 +10339,7 @@
       <c r="F38" s="98">
         <v>0.5</v>
       </c>
-      <c r="G38" s="66">
+      <c r="G38" s="34">
         <v>0</v>
       </c>
       <c r="H38" s="34">
@@ -10537,11 +10547,11 @@
       <c r="L39" s="34"/>
       <c r="M39" s="34"/>
       <c r="N39" s="34"/>
-      <c r="O39" s="35">
+      <c r="O39" s="105">
         <f t="shared" si="11"/>
         <v>6.5</v>
       </c>
-      <c r="P39" s="36">
+      <c r="P39" s="104">
         <f>IF(Info!B$10=0,0,SUM(S39:AD39))+IF(Info!B$11=0,0,2*SUM(S39:AD39))+IF(Info!B$12=0,0,SUM(AS39:BD39))</f>
         <v>2</v>
       </c>
@@ -17612,7 +17622,7 @@
         <v>94439</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="10">
@@ -20869,7 +20879,7 @@
         <v>45365</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -21460,7 +21470,7 @@
       </c>
       <c r="J10" s="18"/>
       <c r="L10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -23080,7 +23090,7 @@
         <v>1686</v>
       </c>
       <c r="L10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -23118,7 +23128,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -23224,7 +23234,7 @@
         <v>1920</v>
       </c>
       <c r="L16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -23235,7 +23245,7 @@
         <v>58700</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D17" s="18">
         <v>1894</v>
@@ -23259,7 +23269,7 @@
         <v>1892</v>
       </c>
       <c r="L17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1">
@@ -23294,7 +23304,7 @@
         <v>1874</v>
       </c>
       <c r="L18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -23402,13 +23412,13 @@
         <v>84166</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J23" s="18" t="s">
         <v>73</v>
       </c>
       <c r="L23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -23443,7 +23453,7 @@
         <v>73</v>
       </c>
       <c r="L24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -23472,13 +23482,13 @@
         <v>82201</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J25" s="18">
         <v>1146</v>
       </c>
       <c r="L25" s="103" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
@@ -23507,13 +23517,13 @@
         <v>88706</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>73</v>
       </c>
       <c r="L26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
@@ -23540,7 +23550,7 @@
       </c>
       <c r="J27" s="3"/>
       <c r="L27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">

</xml_diff>